<commit_message>
Delimiters slightly reworked + separate scripts done
</commit_message>
<xml_diff>
--- a/output/concentrations/ds.3p.2eq/data_res.xlsx
+++ b/output/concentrations/ds.3p.2eq/data_res.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
   <si>
     <t>H</t>
   </si>
@@ -31,13 +31,43 @@
     <t>M</t>
   </si>
   <si>
-    <t>k_constants_log10</t>
+    <t>log10.K.</t>
+  </si>
+  <si>
+    <t>3.14</t>
+  </si>
+  <si>
+    <t>1.45</t>
+  </si>
+  <si>
+    <t>2.79</t>
+  </si>
+  <si>
+    <t>-8.9</t>
+  </si>
+  <si>
+    <t>-13.88</t>
   </si>
   <si>
     <t>eq</t>
   </si>
   <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>1e-04</t>
+  </si>
+  <si>
+    <t>0.001</t>
+  </si>
+  <si>
     <t>tot</t>
+  </si>
+  <si>
+    <t>0.005</t>
   </si>
   <si>
     <t>series</t>
@@ -513,28 +543,28 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2">
-        <v>3.14</v>
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3">
-        <v>1.45</v>
+      <c r="A3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4">
-        <v>2.79</v>
+      <c r="A4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5">
-        <v>-8.9</v>
+      <c r="A5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6">
-        <v>-13.88</v>
+      <c r="A6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -552,13 +582,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -572,40 +602,40 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3">
-        <v>0.01</v>
-      </c>
-      <c r="B3">
-        <v>0.02</v>
-      </c>
-      <c r="C3">
-        <v>0.01</v>
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4">
-        <v>0.001</v>
-      </c>
-      <c r="B4">
-        <v>0.02</v>
-      </c>
-      <c r="C4">
-        <v>0.01</v>
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5">
-        <v>0.0001</v>
-      </c>
-      <c r="B5">
-        <v>0.01</v>
-      </c>
-      <c r="C5">
-        <v>0.005</v>
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -632,72 +662,72 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="B2">
-        <v>0.001324326815762943</v>
+        <v>0.001</v>
       </c>
       <c r="C2">
-        <v>0.01</v>
+        <v>0.004860029427680299</v>
       </c>
       <c r="D2">
-        <v>0.01828079897670811</v>
+        <v>0.1380384264602885</v>
       </c>
       <c r="E2">
-        <v>0.0003732460092962083</v>
+        <v>0.0001369742398441712</v>
       </c>
       <c r="F2">
-        <v>1.081409912174609e-05</v>
+        <v>2.996669854007388e-06</v>
       </c>
       <c r="G2">
-        <v>1.258925411794162e-09</v>
+        <v>6.118414548574175e-11</v>
       </c>
       <c r="H2">
-        <v>1.318256738556402e-12</v>
+        <v>1.318256738556401e-13</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3">
+        <v>0.01</v>
+      </c>
+      <c r="B3">
         <v>0.001</v>
       </c>
-      <c r="B3">
-        <v>0.00726784104519944</v>
-      </c>
       <c r="C3">
-        <v>0.01</v>
+        <v>0.004860028892444237</v>
       </c>
       <c r="D3">
-        <v>0.0100324134164283</v>
+        <v>0.01380384264602885</v>
       </c>
       <c r="E3">
-        <v>0.002048355914893331</v>
+        <v>0.0001369742247591694</v>
       </c>
       <c r="F3">
-        <v>0.0003256948118913796</v>
+        <v>2.996669523983508e-06</v>
       </c>
       <c r="G3">
-        <v>1.258925411794164e-08</v>
+        <v>6.118413874751902e-10</v>
       </c>
       <c r="H3">
-        <v>1.318256738556404e-11</v>
+        <v>1.318256738556402e-12</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -705,22 +735,22 @@
         <v>0.0001</v>
       </c>
       <c r="B4">
-        <v>0.007544457667507364</v>
+        <v>0.01</v>
       </c>
       <c r="C4">
-        <v>0.005</v>
+        <v>0.003721593866991905</v>
       </c>
       <c r="D4">
-        <v>0.001041425064918975</v>
+        <v>0.001380384264602885</v>
       </c>
       <c r="E4">
-        <v>0.001063158535787499</v>
+        <v>0.001048887663182846</v>
       </c>
       <c r="F4">
-        <v>0.0001754793658933968</v>
+        <v>0.0002294716177345554</v>
       </c>
       <c r="G4">
-        <v>6.294627058970815e-08</v>
+        <v>4.68520909153343e-08</v>
       </c>
       <c r="H4">
         <v>1.3182567385564e-10</v>
@@ -741,85 +771,85 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B2">
-        <v>2.878004827005217</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>6.621634078814714</v>
+        <v>100</v>
       </c>
       <c r="D2">
-        <v>91.40399488354055</v>
+        <v>13803.84264602885</v>
       </c>
       <c r="E2">
-        <v>1.866230046481041</v>
+        <v>13.69742398441712</v>
       </c>
       <c r="F2">
-        <v>0.1081409912174609</v>
+        <v>0.5993339708014775</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B3">
-        <v>2.138594579705729</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>36.3392052259972</v>
+        <v>100</v>
       </c>
       <c r="D3">
-        <v>50.16206708214147</v>
+        <v>1380.384264602885</v>
       </c>
       <c r="E3">
-        <v>10.24177957446665</v>
+        <v>13.69742247591694</v>
       </c>
       <c r="F3">
-        <v>3.256948118913795</v>
+        <v>0.5993339047967016</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B4">
-        <v>2.122371973976437</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>75.44457667507363</v>
+        <v>100</v>
       </c>
       <c r="D4">
-        <v>10.41425064918975</v>
+        <v>13.80384264602885</v>
       </c>
       <c r="E4">
-        <v>10.63158535787499</v>
+        <v>10.48887663182846</v>
       </c>
       <c r="F4">
-        <v>3.509587317867935</v>
+        <v>4.589432354691109</v>
       </c>
     </row>
   </sheetData>
@@ -846,7 +876,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -854,10 +884,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1.07552855510562e-14</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>3.985626230093575e-10</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -865,10 +895,10 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>3.038264084764819e-13</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>3.985687778082503e-10</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -876,10 +906,10 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>6.29704621779581e-16</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>2.211772431870429e-16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>